<commit_message>
aanpassingen word en excel doc
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403FBD6-0F65-4242-B4B9-407296B98E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A63152-1AF5-4055-B5A9-063F92A91079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30990" yWindow="-14760" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>zien op welke branch we ons bevinden en of deze al dan niet up to date is met de origin/master branch. We kunnen ook zien welke files in welke stage zijn (committed, staged of modified)</t>
   </si>
   <si>
-    <t>korte versie van status (M: modified, A: new file added to staging area, ??: new file untracked by GIT)</t>
-  </si>
-  <si>
     <t>Welke aanpassingen heb ik gedaan maar niet gestaged</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>git checkout master</t>
   </si>
   <si>
-    <t>checkout:uitchecken naar een andere branch -b: dit wilt zeggen dat we willen uitchecken nr een nieuwe branch</t>
-  </si>
-  <si>
     <t>HEAD verwijst terug nr master branch</t>
   </si>
   <si>
@@ -306,9 +300,6 @@
     <t>gelijk aan git reset: moves changes back to the workin directory</t>
   </si>
   <si>
-    <t>het verplaatstveranderingen naar de trash ==&gt; opassen!! Veranderingen in working directory of staging area gaan ook verloren</t>
-  </si>
-  <si>
     <t>git reset --mixed &lt;commit-id&gt;</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>Repo clonen naar ander apparaat van GITHUB</t>
   </si>
   <si>
-    <t>git config --global core.editor "code --wait --new-window"</t>
-  </si>
-  <si>
     <t>VS code als gloable editor</t>
   </si>
   <si>
@@ -345,9 +333,6 @@
     <t>git fetch</t>
   </si>
   <si>
-    <t>brengt veranderingen in de remote repo dat  nieuw zijn sinds clone naar lokale repo</t>
-  </si>
-  <si>
     <t>git pull</t>
   </si>
   <si>
@@ -387,9 +372,6 @@
     <t xml:space="preserve">creeert pointer (lightweight tag) met naam [naam] naar branch [branch] </t>
   </si>
   <si>
-    <t>git tag -a v0.1 -m "1.0 Release"  3a06a16</t>
-  </si>
-  <si>
     <t>annotated tag met naam v0.1 en message "1.0 release" naar commit 3aO6a16</t>
   </si>
   <si>
@@ -400,6 +382,30 @@
   </si>
   <si>
     <t>Als we de rm --cashed gebruiken, en er dus een untracked bestand is, en we willen veranderen van branch, zou dit bestand overschreven worden, we kunnen verwijderen of terug laten tracken met git add. Indien we dit niet willen, kunnen we deze aanpassing stashen. Dit doen we door eerst git add . te gebruiken en achteraf git stash, Dit wordt dan opgeslagen als een WIP (work in progress)</t>
+  </si>
+  <si>
+    <t>het verplaatst veranderingen naar de trash ==&gt; opassen!! Veranderingen in working directory of staging area gaan 
+ook verloren</t>
+  </si>
+  <si>
+    <t>git config --global core.editor "code
+ --wait --new-window"</t>
+  </si>
+  <si>
+    <t>checkout:uitchecken naar een andere branch -b: dit wilt zeggen dat we willen uitchecken nr een 
+nieuwe branch</t>
+  </si>
+  <si>
+    <t>korte versie van status (M: modified, A: new file added to staging area, ??: 
+new file untracked by GIT)</t>
+  </si>
+  <si>
+    <t>brengt veranderingen in de remote repo dat  nieuw zijn sinds clone naar
+ lokale repo</t>
+  </si>
+  <si>
+    <t>git tag -a v0.1 -m "1.0 Release"
+  3a06a16</t>
   </si>
 </sst>
 </file>
@@ -543,17 +549,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -921,7 +927,7 @@
       <c r="C3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -933,9 +939,9 @@
         <v>44776</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -947,9 +953,9 @@
         <v>44777</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="22"/>
+        <v>89</v>
+      </c>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -1671,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268595DD-CE12-47DD-B2E7-8F8034F6F3A9}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,7 +1715,7 @@
       <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>44777</v>
       </c>
     </row>
@@ -1720,7 +1726,7 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>44778</v>
       </c>
     </row>
@@ -1809,14 +1815,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6478BB-0DED-4932-9D76-061110FF905B}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="A1:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="126.77734375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="28" style="4" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +1837,7 @@
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1839,7 +1845,7 @@
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1847,7 +1853,7 @@
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1855,7 +1861,7 @@
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1863,7 +1869,7 @@
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1871,7 +1877,7 @@
       <c r="A7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1879,8 +1885,8 @@
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>100</v>
+      <c r="B8" s="17" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1891,292 +1897,292 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>42</v>
+      <c r="B10" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="18" t="s">
         <v>63</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="18" t="s">
         <v>65</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>68</v>
+        <v>94</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="18" t="s">
         <v>82</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>95</v>
+      <c r="B38" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>104</v>
+        <v>98</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
word doc af, excel updated
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A63152-1AF5-4055-B5A9-063F92A91079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115DDFA-F72C-4F4F-A848-040D5BCBC027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="123">
   <si>
     <t>maandag</t>
   </si>
@@ -407,12 +407,175 @@
     <t>git tag -a v0.1 -m "1.0 Release"
   3a06a16</t>
   </si>
+  <si>
+    <t>read the doc giunio send me</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Google Cloud SDK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Python</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+gitflow
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PyCharm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>You should enable 2FA authentication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I would advise you to set up an SSH connection to Github</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">check alles in datalake chat, install: </t>
+  </si>
+  <si>
+    <t>Google Cloud Platform: Introduction, Getting Started</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform: VM's in the cloud, Storage in the cloud</t>
+  </si>
+  <si>
+    <t>Google Cloud platform: Containers in the cloud</t>
+  </si>
+  <si>
+    <t>Kubernetes and Docker Containers, Applications in the cloud</t>
+  </si>
+  <si>
+    <t>Developing, Deploying and Monitoring in the cloud, Big Data and Machine learning in the cloud + Installing necessary software (GitFlow, Python, Pip, Google cloud SDK, PyCharm), configur 2FA auth, Setup SSH with GitHub</t>
+  </si>
+  <si>
+    <t>Tutorial  Getting started with GitHub + begin GCP tutorial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +612,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +642,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,13 +680,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -559,6 +734,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -877,20 +1058,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B364332-1EA7-4B6F-A67A-38251FB0CD78}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="184.33203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="157.21875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="198.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="157.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -904,760 +1085,778 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>44774</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>44775</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>44776</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>44777</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>44778</v>
       </c>
+      <c r="C6" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>44779</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>44780</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>44781</v>
       </c>
+      <c r="C9" s="9" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>44782</v>
       </c>
+      <c r="C10" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>44783</v>
       </c>
+      <c r="C11" s="9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>44784</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>44785</v>
       </c>
+      <c r="C13" s="9" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>44786</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>44787</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="23">
         <v>44788</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>44789</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>44790</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>44791</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>44792</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>44793</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>44794</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="8">
         <v>44795</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>44796</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>44797</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>44798</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="8">
         <v>44799</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>44800</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>44801</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="8">
         <v>44802</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="8">
         <v>44803</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="8">
         <v>44804</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>44805</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>44806</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>44807</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>44808</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="8">
         <v>44809</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>44810</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>44811</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>44812</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="8">
         <v>44813</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <v>44814</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <v>44815</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="8">
         <v>44816</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="8">
         <v>44817</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="8">
         <v>44818</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="8">
         <v>44819</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="8">
         <v>44820</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <v>44821</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <v>44822</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="8">
         <v>44823</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="8">
         <v>44824</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="8">
         <v>44825</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="8">
         <v>44826</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="8">
         <v>44827</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <v>44828</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <v>44829</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="8">
         <v>44830</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="8">
         <v>44831</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="8">
         <v>44832</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="8">
         <v>44833</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="8">
         <v>44834</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <v>44835</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <v>44836</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B65" s="8">
         <v>44837</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="8">
         <v>44838</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="8">
         <v>44839</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="8">
         <v>44840</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="8">
         <v>44841</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="6">
         <v>44842</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="6">
         <v>44843</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="9">
+      <c r="B72" s="8">
         <v>44844</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="8">
         <v>44845</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="8">
         <v>44846</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="8">
         <v>44847</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="8">
         <v>44848</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="6">
         <v>44849</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="6">
         <v>44850</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B79" s="8">
         <v>44851</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B80" s="8">
         <v>44852</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="9">
+      <c r="B81" s="8">
         <v>44853</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B82" s="8">
         <v>44854</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B83" s="8">
         <v>44855</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B84" s="6">
         <v>44856</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="6">
         <v>44857</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="9">
+      <c r="B86" s="8">
         <v>44858</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="8">
         <v>44859</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88" s="8">
         <v>44860</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="8">
         <v>44861</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="8">
         <v>44862</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91" s="6">
         <v>44863</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B92" s="6">
         <v>44864</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="9">
+      <c r="B93" s="8">
         <v>44865</v>
       </c>
     </row>
@@ -1677,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268595DD-CE12-47DD-B2E7-8F8034F6F3A9}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1693,48 +1892,55 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>44777</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>44778</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:3" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -1821,367 +2027,367 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28" style="4" customWidth="1"/>
-    <col min="2" max="2" width="64.6640625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28" style="3" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="16" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update LOG en toevoeging PDF Workshop
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A115DDFA-F72C-4F4F-A848-040D5BCBC027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22572D49-E238-48B7-B05D-273F72088DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
   <si>
     <t>maandag</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>Tutorial  Getting started with GitHub + begin GCP tutorial</t>
+  </si>
+  <si>
+    <t>installatie wget, Installatie Gitflow, beginnen workshop</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1062,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,15 +1247,18 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="8">
         <v>44789</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>44790</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1290,7 @@
         <v>44793</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>44794</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1306,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
@@ -1332,7 +1338,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -1877,7 +1883,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
aanpassingen aan Workshop doc en LOG
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A17E0F-7456-4405-BCB2-5BCDF203BB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA58988-A420-46EB-8A75-176EE9041A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
+    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
   <si>
     <t>maandag</t>
   </si>
@@ -142,12 +142,283 @@
   </si>
   <si>
     <t>git push -u origin master</t>
+  </si>
+  <si>
+    <t>In folder van nieuwe repo. Het maakt een master branch</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git status -s</t>
+  </si>
+  <si>
+    <t>git status --short</t>
+  </si>
+  <si>
+    <t>korte versie van status</t>
+  </si>
+  <si>
+    <t>zien op welke branch we ons bevinden en of deze al dan niet up to date is met de origin/master branch. We kunnen ook zien welke files in welke stage zijn (committed, staged of modified)</t>
+  </si>
+  <si>
+    <t>Welke aanpassingen heb ik gedaan maar niet gestaged</t>
+  </si>
+  <si>
+    <t>git diff --staged</t>
+  </si>
+  <si>
+    <t>Welke aanpassingen heb ik gedaan die staged zijn en dus klaar om te worden committed.
+De aanpassingen staan op de onderste lijn, in de chunk header en chunk changes.
+Chunk header geeft aan welke lijnen werden aangepast: - is oude content, + is nieuwe content</t>
+  </si>
+  <si>
+    <t>git diff</t>
+  </si>
+  <si>
+    <t>shortcut staged area via git add (dus meteen van modified naar committed)</t>
+  </si>
+  <si>
+    <t>git commit -a</t>
+  </si>
+  <si>
+    <t>git commit -a -m "add new txtfile"</t>
+  </si>
+  <si>
+    <t>git log</t>
+  </si>
+  <si>
+    <t>Geeft een overzicht vd geschiednis van de commits</t>
+  </si>
+  <si>
+    <t>git log -5</t>
+  </si>
+  <si>
+    <t>Enkel de laatste 5 commits</t>
+  </si>
+  <si>
+    <t>git log --oneline</t>
+  </si>
+  <si>
+    <t>git log --stat</t>
+  </si>
+  <si>
+    <t>lijst van al de commits dat elk slechts 1 lijn innemen (beter overzicht)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uitebreidere lijst (geeft aan welke files werden aangepast in de commits) </t>
+  </si>
+  <si>
+    <t>git log --patch</t>
+  </si>
+  <si>
+    <t>Geeft al de aanpassingen in de files in elke commit (de diff) =&gt; geruik q om te quitten</t>
+  </si>
+  <si>
+    <t>Met een message (geeft aan wat commit betekent)</t>
+  </si>
+  <si>
+    <t>git rm newFile.txt</t>
+  </si>
+  <si>
+    <t>Zorgen dat git dit bestand niet meer volgt en dat het verwijdert wordt</t>
+  </si>
+  <si>
+    <t>Zorgen dat git dit bestand niet meer volgt maar dat het NIET verwijdert wordt</t>
+  </si>
+  <si>
+    <t>git rm --cached newFile.txt</t>
+  </si>
+  <si>
+    <t>bestand hernamen</t>
+  </si>
+  <si>
+    <t>git mv README.md README</t>
+  </si>
+  <si>
+    <t>git checkout master</t>
+  </si>
+  <si>
+    <t>HEAD verwijst terug nr master branch</t>
+  </si>
+  <si>
+    <t>git stash</t>
+  </si>
+  <si>
+    <t>git stash list</t>
+  </si>
+  <si>
+    <t>git stash show</t>
+  </si>
+  <si>
+    <t>git stash pop</t>
+  </si>
+  <si>
+    <t>git merge new_branch</t>
+  </si>
+  <si>
+    <t>nieuwe branch aanmaken</t>
+  </si>
+  <si>
+    <t>lijst van WIP's en hun branch</t>
+  </si>
+  <si>
+    <t>Beter gedetailleerd overzicht van WIPs met de aangepaste bestanden</t>
+  </si>
+  <si>
+    <t>De aanpassing wordt teruggeplaatst in de working directory</t>
+  </si>
+  <si>
+    <t>Merge new_brach into master branch</t>
+  </si>
+  <si>
+    <t>moves changes back into staging area</t>
+  </si>
+  <si>
+    <t>gelijk aan git reset: moves changes back to the workin directory</t>
+  </si>
+  <si>
+    <t>git reset --mixed &lt;commit-id&gt;</t>
+  </si>
+  <si>
+    <t>git reset --soft &lt;commit-id&gt;</t>
+  </si>
+  <si>
+    <t>git reset --hard &lt;commit-id&gt;</t>
+  </si>
+  <si>
+    <t>git push origin master</t>
+  </si>
+  <si>
+    <t>git clone &lt;link-repo&gt;</t>
+  </si>
+  <si>
+    <t>lokale repo nr github</t>
+  </si>
+  <si>
+    <t>Repo clonen naar ander apparaat van GITHUB</t>
+  </si>
+  <si>
+    <t>VS code als gloable editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tutorial van GIT: Basic en Extended commands of everyday GIT  &amp;  Tutorial  Getting started with GitHub</t>
+  </si>
+  <si>
+    <t>Tutorial  Getting started with GitHub</t>
+  </si>
+  <si>
+    <t>git fetch</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Een som van een git fetch en git merge. </t>
+  </si>
+  <si>
+    <t>git branch [naam]</t>
+  </si>
+  <si>
+    <t>git checkout -b [naam]</t>
+  </si>
+  <si>
+    <t>Push locale repo van branch master</t>
+  </si>
+  <si>
+    <t>git push -u origin [branch name]</t>
+  </si>
+  <si>
+    <t>pushes t branch and the -u creates link between local and remote branch</t>
+  </si>
+  <si>
+    <t>git branch -r</t>
+  </si>
+  <si>
+    <t>overzicht van al de lokale branches</t>
+  </si>
+  <si>
+    <t>git tag</t>
+  </si>
+  <si>
+    <t>Geeft een overzicht vd tags</t>
+  </si>
+  <si>
+    <t>git tag [naam] [branch]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creeert pointer (lightweight tag) met naam [naam] naar branch [branch] </t>
+  </si>
+  <si>
+    <t>annotated tag met naam v0.1 en message "1.0 release" naar commit 3aO6a16</t>
+  </si>
+  <si>
+    <t>git push --tags</t>
+  </si>
+  <si>
+    <t>om tags naar github te pushen</t>
+  </si>
+  <si>
+    <t>Als we de rm --cashed gebruiken, en er dus een untracked bestand is, en we willen veranderen van branch, zou dit bestand overschreven worden, we kunnen verwijderen of terug laten tracken met git add. Indien we dit niet willen, kunnen we deze aanpassing stashen. Dit doen we door eerst git add . te gebruiken en achteraf git stash, Dit wordt dan opgeslagen als een WIP (work in progress)</t>
+  </si>
+  <si>
+    <t>het verplaatst veranderingen naar de trash ==&gt; opassen!! Veranderingen in working directory of staging area gaan 
+ook verloren</t>
+  </si>
+  <si>
+    <t>git config --global core.editor "code
+ --wait --new-window"</t>
+  </si>
+  <si>
+    <t>checkout:uitchecken naar een andere branch -b: dit wilt zeggen dat we willen uitchecken nr een 
+nieuwe branch</t>
+  </si>
+  <si>
+    <t>korte versie van status (M: modified, A: new file added to staging area, ??: 
+new file untracked by GIT)</t>
+  </si>
+  <si>
+    <t>brengt veranderingen in de remote repo dat  nieuw zijn sinds clone naar
+ lokale repo</t>
+  </si>
+  <si>
+    <t>git tag -a v0.1 -m "1.0 Release"
+  3a06a16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check alles in datalake chat, install: </t>
+  </si>
+  <si>
+    <t>Google Cloud Platform: Introduction, Getting Started</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform: VM's in the cloud, Storage in the cloud</t>
+  </si>
+  <si>
+    <t>Google Cloud platform: Containers in the cloud</t>
+  </si>
+  <si>
+    <t>Kubernetes and Docker Containers, Applications in the cloud</t>
+  </si>
+  <si>
+    <t>Developing, Deploying and Monitoring in the cloud, Big Data and Machine learning in the cloud + Installing necessary software (GitFlow, Python, Pip, Google cloud SDK, PyCharm), configur 2FA auth, Setup SSH with GitHub</t>
+  </si>
+  <si>
+    <t>Tutorial  Getting started with GitHub + begin GCP tutorial</t>
+  </si>
+  <si>
+    <t>installatie wget, Installatie Gitflow, beginnen workshop: Cloud Storage, Big Query</t>
+  </si>
+  <si>
+    <t>Google Cloud SDK,Python,pip,git,gitflow,PyCharm,You should enable 2FA authentication,I would advise you to set up an SSH connection to Github</t>
+  </si>
+  <si>
+    <t>Workshop Cloud Functions en Data studio</t>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -162,423 +433,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> aan de hand van namespace pckages en aan de hand van het setuptools package. Intro Tutorial van GIT: Get up and running with GIT</t>
+      <t xml:space="preserve"> aan de hand van namespace packages en aan de hand van het setuptools package. Intro Tutorial van GIT: Get up and running with GIT</t>
     </r>
   </si>
   <si>
-    <t>In folder van nieuwe repo. Het maakt een master branch</t>
-  </si>
-  <si>
-    <t>git status</t>
-  </si>
-  <si>
-    <t>git status -s</t>
-  </si>
-  <si>
-    <t>git status --short</t>
-  </si>
-  <si>
-    <t>korte versie van status</t>
-  </si>
-  <si>
-    <t>zien op welke branch we ons bevinden en of deze al dan niet up to date is met de origin/master branch. We kunnen ook zien welke files in welke stage zijn (committed, staged of modified)</t>
-  </si>
-  <si>
-    <t>Welke aanpassingen heb ik gedaan maar niet gestaged</t>
-  </si>
-  <si>
-    <t>git diff --staged</t>
-  </si>
-  <si>
-    <t>Welke aanpassingen heb ik gedaan die staged zijn en dus klaar om te worden committed.
-De aanpassingen staan op de onderste lijn, in de chunk header en chunk changes.
-Chunk header geeft aan welke lijnen werden aangepast: - is oude content, + is nieuwe content</t>
-  </si>
-  <si>
-    <t>git diff</t>
-  </si>
-  <si>
-    <t>shortcut staged area via git add (dus meteen van modified naar committed)</t>
-  </si>
-  <si>
-    <t>git commit -a</t>
-  </si>
-  <si>
-    <t>git commit -a -m "add new txtfile"</t>
-  </si>
-  <si>
-    <t>git log</t>
-  </si>
-  <si>
-    <t>Geeft een overzicht vd geschiednis van de commits</t>
-  </si>
-  <si>
-    <t>git log -5</t>
-  </si>
-  <si>
-    <t>Enkel de laatste 5 commits</t>
-  </si>
-  <si>
-    <t>git log --oneline</t>
-  </si>
-  <si>
-    <t>git log --stat</t>
-  </si>
-  <si>
-    <t>lijst van al de commits dat elk slechts 1 lijn innemen (beter overzicht)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uitebreidere lijst (geeft aan welke files werden aangepast in de commits) </t>
-  </si>
-  <si>
-    <t>git log --patch</t>
-  </si>
-  <si>
-    <t>Geeft al de aanpassingen in de files in elke commit (de diff) =&gt; geruik q om te quitten</t>
-  </si>
-  <si>
-    <t>Met een message (geeft aan wat commit betekent)</t>
-  </si>
-  <si>
-    <t>git rm newFile.txt</t>
-  </si>
-  <si>
-    <t>Zorgen dat git dit bestand niet meer volgt en dat het verwijdert wordt</t>
-  </si>
-  <si>
-    <t>Zorgen dat git dit bestand niet meer volgt maar dat het NIET verwijdert wordt</t>
-  </si>
-  <si>
-    <t>git rm --cached newFile.txt</t>
-  </si>
-  <si>
-    <t>bestand hernamen</t>
-  </si>
-  <si>
-    <t>git mv README.md README</t>
-  </si>
-  <si>
-    <t>git checkout master</t>
-  </si>
-  <si>
-    <t>HEAD verwijst terug nr master branch</t>
-  </si>
-  <si>
-    <t>git stash</t>
-  </si>
-  <si>
-    <t>git stash list</t>
-  </si>
-  <si>
-    <t>git stash show</t>
-  </si>
-  <si>
-    <t>git stash pop</t>
-  </si>
-  <si>
-    <t>git merge new_branch</t>
-  </si>
-  <si>
-    <t>nieuwe branch aanmaken</t>
-  </si>
-  <si>
-    <t>lijst van WIP's en hun branch</t>
-  </si>
-  <si>
-    <t>Beter gedetailleerd overzicht van WIPs met de aangepaste bestanden</t>
-  </si>
-  <si>
-    <t>De aanpassing wordt teruggeplaatst in de working directory</t>
-  </si>
-  <si>
-    <t>Merge new_brach into master branch</t>
-  </si>
-  <si>
-    <t>moves changes back into staging area</t>
-  </si>
-  <si>
-    <t>gelijk aan git reset: moves changes back to the workin directory</t>
-  </si>
-  <si>
-    <t>git reset --mixed &lt;commit-id&gt;</t>
-  </si>
-  <si>
-    <t>git reset --soft &lt;commit-id&gt;</t>
-  </si>
-  <si>
-    <t>git reset --hard &lt;commit-id&gt;</t>
-  </si>
-  <si>
-    <t>git push origin master</t>
-  </si>
-  <si>
-    <t>git clone &lt;link-repo&gt;</t>
-  </si>
-  <si>
-    <t>lokale repo nr github</t>
-  </si>
-  <si>
-    <t>Repo clonen naar ander apparaat van GITHUB</t>
-  </si>
-  <si>
-    <t>VS code als gloable editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tutorial van GIT: Basic en Extended commands of everyday GIT  &amp;  Tutorial  Getting started with GitHub</t>
-  </si>
-  <si>
-    <t>Tutorial  Getting started with GitHub</t>
-  </si>
-  <si>
-    <t>git fetch</t>
-  </si>
-  <si>
-    <t>git pull</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Een som van een git fetch en git merge. </t>
-  </si>
-  <si>
-    <t>git branch [naam]</t>
-  </si>
-  <si>
-    <t>git checkout -b [naam]</t>
-  </si>
-  <si>
-    <t>Push locale repo van branch master</t>
-  </si>
-  <si>
-    <t>git push -u origin [branch name]</t>
-  </si>
-  <si>
-    <t>pushes t branch and the -u creates link between local and remote branch</t>
-  </si>
-  <si>
-    <t>git branch -r</t>
-  </si>
-  <si>
-    <t>overzicht van al de lokale branches</t>
-  </si>
-  <si>
-    <t>git tag</t>
-  </si>
-  <si>
-    <t>Geeft een overzicht vd tags</t>
-  </si>
-  <si>
-    <t>git tag [naam] [branch]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">creeert pointer (lightweight tag) met naam [naam] naar branch [branch] </t>
-  </si>
-  <si>
-    <t>annotated tag met naam v0.1 en message "1.0 release" naar commit 3aO6a16</t>
-  </si>
-  <si>
-    <t>git push --tags</t>
-  </si>
-  <si>
-    <t>om tags naar github te pushen</t>
-  </si>
-  <si>
-    <t>Als we de rm --cashed gebruiken, en er dus een untracked bestand is, en we willen veranderen van branch, zou dit bestand overschreven worden, we kunnen verwijderen of terug laten tracken met git add. Indien we dit niet willen, kunnen we deze aanpassing stashen. Dit doen we door eerst git add . te gebruiken en achteraf git stash, Dit wordt dan opgeslagen als een WIP (work in progress)</t>
-  </si>
-  <si>
-    <t>het verplaatst veranderingen naar de trash ==&gt; opassen!! Veranderingen in working directory of staging area gaan 
-ook verloren</t>
-  </si>
-  <si>
-    <t>git config --global core.editor "code
- --wait --new-window"</t>
-  </si>
-  <si>
-    <t>checkout:uitchecken naar een andere branch -b: dit wilt zeggen dat we willen uitchecken nr een 
-nieuwe branch</t>
-  </si>
-  <si>
-    <t>korte versie van status (M: modified, A: new file added to staging area, ??: 
-new file untracked by GIT)</t>
-  </si>
-  <si>
-    <t>brengt veranderingen in de remote repo dat  nieuw zijn sinds clone naar
- lokale repo</t>
-  </si>
-  <si>
-    <t>git tag -a v0.1 -m "1.0 Release"
-  3a06a16</t>
-  </si>
-  <si>
-    <t>read the doc giunio send me</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Google Cloud SDK</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Python</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>git</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-gitflow
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PyCharm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>You should enable 2FA authentication</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>I would advise you to set up an SSH connection to Github</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">check alles in datalake chat, install: </t>
-  </si>
-  <si>
-    <t>Google Cloud Platform: Introduction, Getting Started</t>
-  </si>
-  <si>
-    <t>Google Cloud Platform: VM's in the cloud, Storage in the cloud</t>
-  </si>
-  <si>
-    <t>Google Cloud platform: Containers in the cloud</t>
-  </si>
-  <si>
-    <t>Kubernetes and Docker Containers, Applications in the cloud</t>
-  </si>
-  <si>
-    <t>Developing, Deploying and Monitoring in the cloud, Big Data and Machine learning in the cloud + Installing necessary software (GitFlow, Python, Pip, Google cloud SDK, PyCharm), configur 2FA auth, Setup SSH with GitHub</t>
-  </si>
-  <si>
-    <t>Tutorial  Getting started with GitHub + begin GCP tutorial</t>
-  </si>
-  <si>
-    <t>installatie wget, Installatie Gitflow, beginnen workshop</t>
+    <t>De workshop</t>
+  </si>
+  <si>
+    <t>CloudStorage, BigQuery,CloudFunctions, DataStudio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,14 +479,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -738,11 +599,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1061,16 +925,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B364332-1EA7-4B6F-A67A-38251FB0CD78}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="198.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="157.21875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="216" style="9" customWidth="1"/>
+    <col min="4" max="4" width="115.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1109,7 +973,7 @@
         <v>44775</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
@@ -1123,7 +987,7 @@
         <v>44776</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>13</v>
@@ -1137,7 +1001,7 @@
         <v>44777</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="18"/>
     </row>
@@ -1149,7 +1013,7 @@
         <v>44778</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,7 +1040,7 @@
         <v>44781</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1187,7 +1051,7 @@
         <v>44782</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,7 +1062,7 @@
         <v>44783</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1209,7 +1073,7 @@
         <v>44784</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1220,7 +1084,7 @@
         <v>44785</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1240,10 +1104,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>44788</v>
       </c>
     </row>
@@ -1255,7 +1119,7 @@
         <v>44789</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1264,6 +1128,9 @@
       </c>
       <c r="B18" s="8">
         <v>44790</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1883,7 +1750,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,9 +1787,7 @@
       <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="17">
-        <v>44777</v>
-      </c>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -1931,21 +1796,22 @@
       <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17">
-        <v>44778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>115</v>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2027,8 +1893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6478BB-0DED-4932-9D76-061110FF905B}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2066,7 +1932,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2098,303 +1964,303 @@
         <v>34</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>98</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FastAPI toegevoegd, LOG update
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA58988-A420-46EB-8A75-176EE9041A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A983D82E-9168-4110-A651-80A12A595C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4530" yWindow="-16320" windowWidth="38640" windowHeight="15840" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
+    <workbookView xWindow="-33330" yWindow="-15150" windowWidth="29040" windowHeight="15840" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="127">
   <si>
     <t>maandag</t>
   </si>
@@ -411,9 +411,6 @@
   </si>
   <si>
     <t>Google Cloud SDK,Python,pip,git,gitflow,PyCharm,You should enable 2FA authentication,I would advise you to set up an SSH connection to Github</t>
-  </si>
-  <si>
-    <t>Workshop Cloud Functions en Data studio</t>
   </si>
   <si>
     <r>
@@ -441,6 +438,12 @@
   </si>
   <si>
     <t>CloudStorage, BigQuery,CloudFunctions, DataStudio</t>
+  </si>
+  <si>
+    <t>Explore Python Libraries: FastAPI | Pluralsight</t>
+  </si>
+  <si>
+    <t>Workshop Cloud Functions en Data studio,  pluralsight skill: Explore Python Libraries: FastAPI</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,6 +611,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -926,7 +930,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +977,7 @@
         <v>44775</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
@@ -1111,7 +1115,7 @@
         <v>44788</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
@@ -1122,7 +1126,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1130,10 +1134,13 @@
         <v>44790</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1141,7 +1148,7 @@
         <v>44791</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1149,7 +1156,7 @@
         <v>44792</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
@@ -1157,7 +1164,7 @@
         <v>44793</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>44794</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1180,7 @@
         <v>44795</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
@@ -1181,7 +1188,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1189,7 +1196,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>44798</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>44799</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>44800</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1228,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>44802</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
@@ -1237,7 +1244,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -1739,9 +1746,10 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{EA86F495-7638-4378-8948-D1A4058B5E40}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{705AFD63-C4DE-4887-AA25-4B5DF1B0AAF8}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{67580AED-9487-4687-8960-0FC2AFCCCA6D}"/>
+    <hyperlink ref="D18" r:id="rId4" display="https://app.pluralsight.com/guides/explore-python-libraries:-fastapi" xr:uid="{3A9644FF-0358-4913-87EC-76A1A746EBF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1808,10 +1816,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
         <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add marika report and update log
</commit_message>
<xml_diff>
--- a/LOG_STAGE_RBFA.xlsx
+++ b/LOG_STAGE_RBFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mivel.ext\Desktop\RBFA_FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A983D82E-9168-4110-A651-80A12A595C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48260821-C92D-4828-AF4F-5CFFA2F8AEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33330" yWindow="-15150" windowWidth="29040" windowHeight="15840" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35F0B19B-BFDF-490C-91EA-19571633B7A9}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="145">
   <si>
     <t>maandag</t>
   </si>
@@ -93,10 +93,6 @@
   </si>
   <si>
     <t>google cloud platform</t>
-  </si>
-  <si>
-    <t>PC ontvangen, contract getekend PC overeenkomst, VPN geïnstalleerd, dagelijkse meeting 10u30-11u IT team, TO DO opgesteld eerste week met Giunio, SLACK geïnstalleerd, Plural Sights credentials
---&gt; beginnen met tutorial voor python core organiseren van programma's</t>
   </si>
   <si>
     <t>link</t>
@@ -302,9 +298,6 @@
     <t>VS code als gloable editor</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tutorial van GIT: Basic en Extended commands of everyday GIT  &amp;  Tutorial  Getting started with GitHub</t>
-  </si>
-  <si>
     <t>Tutorial  Getting started with GitHub</t>
   </si>
   <si>
@@ -401,16 +394,102 @@
     <t>Kubernetes and Docker Containers, Applications in the cloud</t>
   </si>
   <si>
-    <t>Developing, Deploying and Monitoring in the cloud, Big Data and Machine learning in the cloud + Installing necessary software (GitFlow, Python, Pip, Google cloud SDK, PyCharm), configur 2FA auth, Setup SSH with GitHub</t>
-  </si>
-  <si>
     <t>Tutorial  Getting started with GitHub + begin GCP tutorial</t>
   </si>
   <si>
-    <t>installatie wget, Installatie Gitflow, beginnen workshop: Cloud Storage, Big Query</t>
-  </si>
-  <si>
     <t>Google Cloud SDK,Python,pip,git,gitflow,PyCharm,You should enable 2FA authentication,I would advise you to set up an SSH connection to Github</t>
+  </si>
+  <si>
+    <t>De workshop</t>
+  </si>
+  <si>
+    <t>CloudStorage, BigQuery,CloudFunctions, DataStudio</t>
+  </si>
+  <si>
+    <t>Explore Python Libraries: FastAPI | Pluralsight</t>
+  </si>
+  <si>
+    <t>handtekening</t>
+  </si>
+  <si>
+    <t>Workshop Cloud Functions en Data studio,  pluralsight tutorial: Explore Python Libraries: FastAPI</t>
+  </si>
+  <si>
+    <t>Deploying frist app with App Engine: solving problems with the guvicorn library</t>
+  </si>
+  <si>
+    <t>Developing, Deploying and Monitoring in the cloud, Big Data and Machine learning in the cloud + Installing necessary software (GitFlow, Python,Pip,Google cloud SDK, PyCharm), configur 2FA auth, Setup SSH with GitHub</t>
+  </si>
+  <si>
+    <t>branch voor elke feature --&gt; development</t>
+  </si>
+  <si>
+    <t>af de master branch blijven</t>
+  </si>
+  <si>
+    <t>invert pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make changes </t>
+  </si>
+  <si>
+    <t>pre commit</t>
+  </si>
+  <si>
+    <t>API design to insert timestamp in a BigQuery table</t>
+  </si>
+  <si>
+    <t>API design to insert file including a timestamp in a cloud storage bucket</t>
+  </si>
+  <si>
+    <t>creating virtual environment, chaneg branches so that dev branch has multiple feature branches, file with timestamp in a cloud storage bucket</t>
+  </si>
+  <si>
+    <t>Create and update entity in Datastore using a FastAPI API. Create pull requests and merge different branches</t>
+  </si>
+  <si>
+    <t>revert commits in development branch, make changes in branch to insert row to bigquery table, look up what isort &amp; black pre-commits do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git reset </t>
+  </si>
+  <si>
+    <t>verwijder latere commits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git revert --hard </t>
+  </si>
+  <si>
+    <r>
+      <t>git </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>reset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF444444"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> --hard f414f31 gaat terug naar commit f414f31</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">received laptop,signed contract for received hardware, VPN installation, daily meeting 10u30-11u IT team, TO DO list created, SLACK installed, Plural Sights credentials--&gt; started with tutorial for python core organisation </t>
+  </si>
+  <si>
+    <t>installation wget, Installation Gitflow, started workshop: Cloud Storage, Big Query</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tutorial of GIT: Basic en Extended commands of everyday GIT  &amp;  Tutorial  Getting started with GitHub</t>
   </si>
   <si>
     <r>
@@ -420,7 +499,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Snappen van plugins</t>
+      <t>getting plugins with</t>
     </r>
     <r>
       <rPr>
@@ -430,27 +509,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> aan de hand van namespace packages en aan de hand van het setuptools package. Intro Tutorial van GIT: Get up and running with GIT</t>
+      <t xml:space="preserve"> namespace packages and with setuptools package. Intro Tutorial of GIT: Get up and running with GIT</t>
     </r>
   </si>
   <si>
-    <t>De workshop</t>
-  </si>
-  <si>
-    <t>CloudStorage, BigQuery,CloudFunctions, DataStudio</t>
-  </si>
-  <si>
-    <t>Explore Python Libraries: FastAPI | Pluralsight</t>
-  </si>
-  <si>
-    <t>Workshop Cloud Functions en Data studio,  pluralsight skill: Explore Python Libraries: FastAPI</t>
+    <t>Isort &amp; black pre-commits added to the branch for inserting a timestamp in bigquery</t>
+  </si>
+  <si>
+    <t>code old changes into new featuresn make PR &amp; merge if reviewed. Do the cron job ==&gt; workshop done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +562,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF444444"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -519,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -542,12 +630,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -568,9 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,7 +733,36 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -927,829 +1078,962 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B364332-1EA7-4B6F-A67A-38251FB0CD78}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="216" style="9" customWidth="1"/>
-    <col min="4" max="4" width="115.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="129.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="113.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="25">
         <v>44774</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="25">
         <v>44775</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="25">
         <v>44776</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="25">
         <v>44777</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="25">
         <v>44778</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="26">
         <v>44779</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="26">
         <v>44780</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="25">
         <v>44781</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="25">
         <v>44782</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="25">
         <v>44783</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="25">
         <v>44784</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="25">
         <v>44785</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="26">
         <v>44786</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="26">
         <v>44787</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="27">
         <v>44788</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="25">
         <v>44789</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="25">
         <v>44790</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="25">
         <v>44791</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="25">
         <v>44792</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="26">
         <v>44793</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="26">
         <v>44794</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="25">
         <v>44795</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="25">
         <v>44796</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="25">
         <v>44797</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="29"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="25">
         <v>44798</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="25">
         <v>44799</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="26">
         <v>44800</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="26">
         <v>44801</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="30"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="25">
         <v>44802</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="28"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="25">
         <v>44803</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="25">
         <v>44804</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" s="29"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="25">
         <v>44805</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" s="29"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="25">
         <v>44806</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34" s="29"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="26">
         <v>44807</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="26">
         <v>44808</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="25">
         <v>44809</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="25">
         <v>44810</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D38" s="29"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="25">
         <v>44811</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D39" s="29"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="25">
         <v>44812</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D40" s="29"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="25">
         <v>44813</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D41" s="29"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="26">
         <v>44814</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D42" s="29"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="26">
         <v>44815</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D43" s="30"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="25">
         <v>44816</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D44" s="28"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="25">
         <v>44817</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D45" s="29"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="25">
         <v>44818</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46" s="29"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="25">
         <v>44819</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D47" s="29"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="25">
         <v>44820</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D48" s="29"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="26">
         <v>44821</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D49" s="29"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="26">
         <v>44822</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D50" s="29"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" s="25">
         <v>44823</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D51" s="29"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="25">
         <v>44824</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D52" s="29"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="25">
         <v>44825</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D53" s="29"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="25">
         <v>44826</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54" s="29"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="25">
         <v>44827</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55" s="29"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="26">
         <v>44828</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D56" s="29"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="26">
         <v>44829</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57" s="30"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="8">
+      <c r="B58" s="25">
         <v>44830</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58" s="28"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="25">
         <v>44831</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59" s="29"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="25">
         <v>44832</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60" s="29"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="8">
+      <c r="B61" s="25">
         <v>44833</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D61" s="29"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="25">
         <v>44834</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D62" s="29"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="26">
         <v>44835</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63" s="29"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="26">
         <v>44836</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D64" s="29"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="25">
         <v>44837</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D65" s="29"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="25">
         <v>44838</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D66" s="29"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B67" s="8">
+      <c r="B67" s="25">
         <v>44839</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D67" s="29"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="8">
+      <c r="B68" s="25">
         <v>44840</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68" s="29"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="8">
+      <c r="B69" s="25">
         <v>44841</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D69" s="29"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="26">
         <v>44842</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D70" s="29"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="26">
         <v>44843</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D71" s="30"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="8">
+      <c r="B72" s="25">
         <v>44844</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D72" s="28"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="25">
         <v>44845</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D73" s="29"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="8">
+      <c r="B74" s="25">
         <v>44846</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D74" s="29"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="8">
+      <c r="B75" s="25">
         <v>44847</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D75" s="29"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="8">
+      <c r="B76" s="25">
         <v>44848</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D76" s="29"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="26">
         <v>44849</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D77" s="29"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="26">
         <v>44850</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D78" s="29"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="8">
+      <c r="B79" s="25">
         <v>44851</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D79" s="29"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="8">
+      <c r="B80" s="25">
         <v>44852</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D80" s="29"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="8">
+      <c r="B81" s="25">
         <v>44853</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D81" s="29"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="25">
         <v>44854</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D82" s="29"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="25">
         <v>44855</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D83" s="29"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="26">
         <v>44856</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D84" s="29"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="26">
         <v>44857</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D85" s="30"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="25">
         <v>44858</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D86" s="28"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="8">
+      <c r="B87" s="25">
         <v>44859</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D87" s="29"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="8">
+      <c r="B88" s="25">
         <v>44860</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D88" s="29"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B89" s="25">
         <v>44861</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D89" s="29"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B90" s="25">
         <v>44862</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D90" s="29"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="26">
         <v>44863</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D91" s="29"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="26">
         <v>44864</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D92" s="29"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="8">
+      <c r="B93" s="25">
         <v>44865</v>
       </c>
+      <c r="D93" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="D86:D93"/>
+    <mergeCell ref="D2:D15"/>
+    <mergeCell ref="D16:D29"/>
+    <mergeCell ref="D30:D43"/>
+    <mergeCell ref="D44:D57"/>
+    <mergeCell ref="D58:D71"/>
+    <mergeCell ref="D72:D85"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{EA86F495-7638-4378-8948-D1A4058B5E40}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{705AFD63-C4DE-4887-AA25-4B5DF1B0AAF8}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{67580AED-9487-4687-8960-0FC2AFCCCA6D}"/>
-    <hyperlink ref="D18" r:id="rId4" display="https://app.pluralsight.com/guides/explore-python-libraries:-fastapi" xr:uid="{3A9644FF-0358-4913-87EC-76A1A746EBF0}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{EA86F495-7638-4378-8948-D1A4058B5E40}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{705AFD63-C4DE-4887-AA25-4B5DF1B0AAF8}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{67580AED-9487-4687-8960-0FC2AFCCCA6D}"/>
+    <hyperlink ref="E18" r:id="rId4" display="https://app.pluralsight.com/guides/explore-python-libraries:-fastapi" xr:uid="{3A9644FF-0358-4913-87EC-76A1A746EBF0}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{A95D37DB-BB8E-47A0-B9AA-5E05BCAB3991}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1758,7 +2042,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,66 +2057,77 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>121</v>
+      <c r="A6" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -1899,376 +2194,392 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6478BB-0DED-4932-9D76-061110FF905B}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" style="3" customWidth="1"/>
-    <col min="2" max="2" width="64.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="21" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>94</v>
+        <v>33</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>110</v>
+        <v>36</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="16" t="s">
         <v>45</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="16" t="s">
         <v>61</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="16" t="s">
         <v>63</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>72</v>
+        <v>90</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>109</v>
+        <v>91</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>106</v>
+        <v>66</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="16" t="s">
         <v>78</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>111</v>
+        <v>87</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>101</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>